<commit_message>
feat(schema): 👷‍♂️ Office schema
</commit_message>
<xml_diff>
--- a/B]_PL-SQL/Oracle Notes/Mastek_Traner_notes/assignments/1]_Normalization Prac/Normalization exercersie.xlsx
+++ b/B]_PL-SQL/Oracle Notes/Mastek_Traner_notes/assignments/1]_Normalization Prac/Normalization exercersie.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="102">
   <si>
     <t>Normalization exercersie 1_31Jan24</t>
   </si>
@@ -304,6 +304,9 @@
     <t>FID -&gt; F_Name, F_phone</t>
   </si>
   <si>
+    <t>Final table list in 3NF:</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Georgia"/>
@@ -396,9 +399,6 @@
     <t>hill</t>
   </si>
   <si>
-    <t>Brime</t>
-  </si>
-  <si>
     <t>CK: (EID, PID) -&gt; (EID, PID, DID, Btime, Ename, Dname, Pname)</t>
   </si>
   <si>
@@ -411,10 +411,10 @@
     <t>pail</t>
   </si>
   <si>
-    <t>emp</t>
-  </si>
-  <si>
-    <t>dept</t>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>department</t>
   </si>
   <si>
     <t>project</t>
@@ -2250,6 +2250,77 @@
       <c r="C46" s="61"/>
       <c r="D46" s="61"/>
     </row>
+    <row r="48">
+      <c r="B48" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="15"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="15"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="15"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:B1"/>
@@ -2297,7 +2368,7 @@
     <row r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2305,7 +2376,7 @@
     <row r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="6"/>
@@ -2313,7 +2384,7 @@
     <row r="7">
       <c r="A7" s="4"/>
       <c r="B7" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2321,7 +2392,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2329,7 +2400,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2337,7 +2408,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2385,25 +2456,25 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="G16" s="62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I16" s="63" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J16" s="63" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K16" s="63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L16" s="63" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M16" s="64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
@@ -2415,19 +2486,19 @@
         <v>10.0</v>
       </c>
       <c r="H17" s="66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I17" s="67">
         <v>1.0</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K17" s="67">
         <v>27.0</v>
       </c>
       <c r="L17" s="66" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M17" s="68">
         <v>4.5</v>
@@ -2442,19 +2513,19 @@
         <v>10.0</v>
       </c>
       <c r="H18" s="70" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I18" s="71">
         <v>5.0</v>
       </c>
       <c r="J18" s="70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K18" s="71">
         <v>25.0</v>
       </c>
       <c r="L18" s="70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M18" s="72">
         <v>3.0</v>
@@ -2469,19 +2540,19 @@
         <v>10.0</v>
       </c>
       <c r="H19" s="66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I19" s="67">
         <v>11.0</v>
       </c>
       <c r="J19" s="66" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K19" s="67">
         <v>22.0</v>
       </c>
       <c r="L19" s="66" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M19" s="68">
         <v>7.0</v>
@@ -2496,19 +2567,19 @@
         <v>14.0</v>
       </c>
       <c r="H20" s="70" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I20" s="71">
         <v>2.0</v>
       </c>
       <c r="J20" s="70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K20" s="71">
         <v>26.0</v>
       </c>
       <c r="L20" s="70" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M20" s="72">
         <v>8.0</v>
@@ -2523,19 +2594,19 @@
         <v>14.0</v>
       </c>
       <c r="H21" s="66" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I21" s="67">
         <v>4.0</v>
       </c>
       <c r="J21" s="66" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K21" s="67">
         <v>21.0</v>
       </c>
       <c r="L21" s="66" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M21" s="68">
         <v>9.0</v>
@@ -2582,34 +2653,34 @@
         <v>45</v>
       </c>
       <c r="G27" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="I27" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="64" t="s">
         <v>73</v>
-      </c>
-      <c r="H27" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="I27" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="J27" s="64" t="s">
-        <v>72</v>
       </c>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="62" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N27" s="64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O27" s="15"/>
       <c r="P27" s="62" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q27" s="63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R27" s="64" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
@@ -2621,13 +2692,13 @@
         <v>1.0</v>
       </c>
       <c r="H28" s="66" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I28" s="67">
         <v>10.0</v>
       </c>
       <c r="J28" s="73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
@@ -2635,7 +2706,7 @@
         <v>27.0</v>
       </c>
       <c r="N28" s="73" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O28" s="15"/>
       <c r="P28" s="65">
@@ -2657,13 +2728,13 @@
         <v>5.0</v>
       </c>
       <c r="H29" s="70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I29" s="71">
         <v>10.0</v>
       </c>
       <c r="J29" s="74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
@@ -2671,7 +2742,7 @@
         <v>25.0</v>
       </c>
       <c r="N29" s="74" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O29" s="15"/>
       <c r="P29" s="69">
@@ -2693,13 +2764,13 @@
         <v>11.0</v>
       </c>
       <c r="H30" s="66" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I30" s="67">
         <v>10.0</v>
       </c>
       <c r="J30" s="73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
@@ -2707,7 +2778,7 @@
         <v>22.0</v>
       </c>
       <c r="N30" s="73" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O30" s="15"/>
       <c r="P30" s="65">
@@ -2727,13 +2798,13 @@
         <v>2.0</v>
       </c>
       <c r="H31" s="70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I31" s="71">
         <v>14.0</v>
       </c>
       <c r="J31" s="74" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
@@ -2761,13 +2832,13 @@
         <v>4.0</v>
       </c>
       <c r="H32" s="66" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I32" s="67">
         <v>14.0</v>
       </c>
       <c r="J32" s="73" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
@@ -2775,7 +2846,7 @@
         <v>21.0</v>
       </c>
       <c r="N32" s="73" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O32" s="15"/>
       <c r="P32" s="65">
@@ -2857,33 +2928,33 @@
     <row r="38">
       <c r="A38" s="4"/>
       <c r="B38" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G38" s="75" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H38" s="63" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I38" s="63" t="s">
         <v>99</v>
       </c>
       <c r="J38" s="15"/>
       <c r="K38" s="76" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L38" s="64" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M38" s="15"/>
       <c r="N38" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O38" s="64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P38" s="15"/>
       <c r="Q38" s="75" t="s">
@@ -2893,7 +2964,7 @@
         <v>101</v>
       </c>
       <c r="S38" s="64" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39">
@@ -2905,7 +2976,7 @@
         <v>1.0</v>
       </c>
       <c r="H39" s="78" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I39" s="79">
         <v>10.0</v>
@@ -2915,14 +2986,14 @@
         <v>10.0</v>
       </c>
       <c r="L39" s="80" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M39" s="15"/>
       <c r="N39" s="65">
         <v>27.0</v>
       </c>
       <c r="O39" s="73" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="P39" s="15"/>
       <c r="Q39" s="65">
@@ -2944,7 +3015,7 @@
         <v>5.0</v>
       </c>
       <c r="H40" s="82" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I40" s="83">
         <v>10.0</v>
@@ -2954,14 +3025,14 @@
         <v>14.0</v>
       </c>
       <c r="L40" s="84" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M40" s="15"/>
       <c r="N40" s="69">
         <v>25.0</v>
       </c>
       <c r="O40" s="74" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="P40" s="15"/>
       <c r="Q40" s="69">
@@ -2983,7 +3054,7 @@
         <v>11.0</v>
       </c>
       <c r="H41" s="78" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I41" s="79">
         <v>10.0</v>
@@ -2996,7 +3067,7 @@
         <v>22.0</v>
       </c>
       <c r="O41" s="73" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P41" s="15"/>
       <c r="Q41" s="65">
@@ -3018,7 +3089,7 @@
         <v>2.0</v>
       </c>
       <c r="H42" s="82" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I42" s="83">
         <v>14.0</v>
@@ -3053,7 +3124,7 @@
         <v>4.0</v>
       </c>
       <c r="H43" s="78" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I43" s="79">
         <v>14.0</v>
@@ -3066,7 +3137,7 @@
         <v>21.0</v>
       </c>
       <c r="O43" s="73" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P43" s="15"/>
       <c r="Q43" s="65">
@@ -3096,6 +3167,75 @@
       <c r="B46" s="61"/>
       <c r="C46" s="61"/>
       <c r="D46" s="61"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="63" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="15"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="15"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="64" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>